<commit_message>
change cavity's permutable_params function, fix names error of a cavity thermal transformation's output, add tolerance matrix to cavity's specs
</commit_message>
<xml_diff>
--- a/Cavity details.xlsx
+++ b/Cavity details.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaeka\Dropbox (Weizmann Institute)\Michael Kali’s files\Home\Research\cavity-design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkali\Dropbox (Weizmann Institute)\Michael Kali’s files\Home\Research\cavity-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717C8ABA-D929-4268-89FE-C463C44C262F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F113CD58-BD32-408E-AF91-7CDF8E712A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{28E137F5-53DE-4F77-89AE-A54727DCF69F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{28E137F5-53DE-4F77-89AE-A54727DCF69F}"/>
   </bookViews>
   <sheets>
-    <sheet name="lens center thicnkess 4.33mm" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Material</t>
   </si>
@@ -63,6 +74,9 @@
     <t>Angle between side rays and surface (degrees)</t>
   </si>
   <si>
+    <t>67.15/88.13</t>
+  </si>
+  <si>
     <t>-</t>
   </si>
   <si>
@@ -100,24 +114,6 @@
   </si>
   <si>
     <t>Veritcal diameter/Height [m]</t>
-  </si>
-  <si>
-    <t>71.33/80.08</t>
-  </si>
-  <si>
-    <t>Right NA</t>
-  </si>
-  <si>
-    <t>Left NA</t>
-  </si>
-  <si>
-    <t>Finesse</t>
-  </si>
-  <si>
-    <t>roundtrip power losses:</t>
-  </si>
-  <si>
-    <t>Free Spectral Range [Hz]:</t>
   </si>
 </sst>
 </file>
@@ -175,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,19 +467,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B50DF3-B8C6-40BE-B318-45B4C91779A8}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -494,7 +490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -508,9 +504,9 @@
         <v>0.30620000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>0.01</v>
@@ -522,9 +518,9 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -536,23 +532,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>2E-3</v>
@@ -564,9 +560,9 @@
         <v>2.4399999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>6.0000000000000001E-3</v>
@@ -580,7 +576,7 @@
         <v>7.3200000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -588,27 +584,27 @@
         <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>1E-4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -622,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -636,9 +632,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>7.4999999999999997E-8</v>
@@ -650,7 +646,7 @@
         <v>7.4999999999999997E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -664,9 +660,9 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
         <v>1.31</v>
@@ -678,9 +674,9 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -692,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -706,9 +702,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -718,46 +714,6 @@
       </c>
       <c r="D17" s="1">
         <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="1">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1">
-        <v>457500000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.0411E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>